<commit_message>
added new requirements to the backlog and updated the product burndown
</commit_message>
<xml_diff>
--- a/documents/Backlog.xlsx
+++ b/documents/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="24000" windowHeight="10260" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="24000" windowHeight="10260"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
   <si>
     <t>Item ID</t>
   </si>
@@ -134,6 +134,45 @@
   </si>
   <si>
     <t>Integrate parts and display a graph</t>
+  </si>
+  <si>
+    <t>Improve input and output UI</t>
+  </si>
+  <si>
+    <t>validation for zipcode</t>
+  </si>
+  <si>
+    <t>New Total</t>
+  </si>
+  <si>
+    <t>As a customer I want to have a boundary for the input of the concrete temperature from 45F to 115F</t>
+  </si>
+  <si>
+    <t>As a customer I want to have 12PM labelled as Noon</t>
+  </si>
+  <si>
+    <t>As a customer I want the tooltips to be displayed near the point on the graph</t>
+  </si>
+  <si>
+    <t>As a customer I want evaporation rates to be rounded to two decimals</t>
+  </si>
+  <si>
+    <t>As a customer I want other people to be included in a project to receive notifications as well</t>
+  </si>
+  <si>
+    <t>As a customer I want low-med-high risk to be displayed over the colors in the graph background</t>
+  </si>
+  <si>
+    <t>As a customer I want to have a page that explains how to use the evaporation rate tool and how it works</t>
+  </si>
+  <si>
+    <t>As a customer I want an indication of what zip code the graph is displaying information about</t>
+  </si>
+  <si>
+    <t>As a customer I want to be able to click a point on the graph to change the variables of the formula</t>
+  </si>
+  <si>
+    <t>As a customer I want to see what concrete temperatures are required to lower the evaporation rate</t>
   </si>
 </sst>
 </file>
@@ -216,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -266,6 +305,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -360,16 +402,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A2:D17" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A2:D17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A2:D27" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A2:D27"/>
   <sortState ref="A4:D25">
     <sortCondition ref="A1:A23"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="Item ID" dataDxfId="9"/>
-    <tableColumn id="2" name="Priority" dataDxfId="8"/>
-    <tableColumn id="3" name="Backlog Item" dataDxfId="7"/>
-    <tableColumn id="4" name="Estimated remaining (person-hours)" dataDxfId="6"/>
+    <tableColumn id="1" name="Item ID" dataDxfId="3"/>
+    <tableColumn id="2" name="Priority" dataDxfId="2"/>
+    <tableColumn id="3" name="Backlog Item" dataDxfId="1"/>
+    <tableColumn id="4" name="Estimated remaining (person-hours)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -389,16 +431,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D22" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D22" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:D22"/>
   <sortState ref="A2:D23">
     <sortCondition ref="A1:A23"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="Item ID" dataDxfId="3"/>
-    <tableColumn id="2" name="Priority" dataDxfId="2"/>
-    <tableColumn id="3" name="Backlog Item" dataDxfId="1"/>
-    <tableColumn id="4" name="Estimated remaining (person-hours)" dataDxfId="0"/>
+    <tableColumn id="1" name="Item ID" dataDxfId="9"/>
+    <tableColumn id="2" name="Priority" dataDxfId="8"/>
+    <tableColumn id="3" name="Backlog Item" dataDxfId="7"/>
+    <tableColumn id="4" name="Estimated remaining (person-hours)" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -667,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,11 +723,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
       <c r="D1" s="14" t="s">
         <v>30</v>
       </c>
@@ -914,16 +956,138 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>22</v>
+      </c>
       <c r="B18" s="1"/>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>23</v>
       </c>
-      <c r="D18" s="1">
+      <c r="B19" s="1"/>
+      <c r="C19" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>24</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>25</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>26</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>27</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>28</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>29</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>30</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>31</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="1">
         <f>SUM(Table13[Estimated remaining (person-hours)])</f>
-        <v>125</v>
-      </c>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -940,7 +1104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -952,12 +1116,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1005,10 +1169,10 @@
       <c r="B5" s="10"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="20"/>
+      <c r="B6" s="21"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
@@ -1038,10 +1202,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,12 +1217,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1113,7 +1277,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1136,12 +1300,49 @@
       </c>
       <c r="D7" s="10">
         <f>SUM(D3:D6)</f>
-        <v>10</v>
-      </c>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="21"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="18"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="18">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1155,7 +1356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="B12" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated the backlog again
</commit_message>
<xml_diff>
--- a/documents/Backlog.xlsx
+++ b/documents/Backlog.xlsx
@@ -402,16 +402,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A2:D27" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A2:D27" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A2:D27"/>
   <sortState ref="A4:D25">
     <sortCondition ref="A1:A23"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="Item ID" dataDxfId="3"/>
-    <tableColumn id="2" name="Priority" dataDxfId="2"/>
-    <tableColumn id="3" name="Backlog Item" dataDxfId="1"/>
-    <tableColumn id="4" name="Estimated remaining (person-hours)" dataDxfId="0"/>
+    <tableColumn id="1" name="Item ID" dataDxfId="9"/>
+    <tableColumn id="2" name="Priority" dataDxfId="8"/>
+    <tableColumn id="3" name="Backlog Item" dataDxfId="7"/>
+    <tableColumn id="4" name="Estimated remaining (person-hours)" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -431,16 +431,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D22" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D22" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D22"/>
   <sortState ref="A2:D23">
     <sortCondition ref="A1:A23"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="Item ID" dataDxfId="9"/>
-    <tableColumn id="2" name="Priority" dataDxfId="8"/>
-    <tableColumn id="3" name="Backlog Item" dataDxfId="7"/>
-    <tableColumn id="4" name="Estimated remaining (person-hours)" dataDxfId="6"/>
+    <tableColumn id="1" name="Item ID" dataDxfId="3"/>
+    <tableColumn id="2" name="Priority" dataDxfId="2"/>
+    <tableColumn id="3" name="Backlog Item" dataDxfId="1"/>
+    <tableColumn id="4" name="Estimated remaining (person-hours)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -701,7 +701,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -712,7 +712,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,7 +960,9 @@
       <c r="A18" s="1">
         <v>22</v>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="1">
+        <v>4</v>
+      </c>
       <c r="C18" s="15" t="s">
         <v>38</v>
       </c>
@@ -972,7 +974,9 @@
       <c r="A19" s="1">
         <v>23</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="1">
+        <v>4</v>
+      </c>
       <c r="C19" s="15" t="s">
         <v>39</v>
       </c>
@@ -984,7 +988,9 @@
       <c r="A20" s="1">
         <v>24</v>
       </c>
-      <c r="B20" s="1"/>
+      <c r="B20" s="1">
+        <v>3</v>
+      </c>
       <c r="C20" s="15" t="s">
         <v>40</v>
       </c>
@@ -996,7 +1002,9 @@
       <c r="A21" s="1">
         <v>25</v>
       </c>
-      <c r="B21" s="1"/>
+      <c r="B21" s="1">
+        <v>3</v>
+      </c>
       <c r="C21" s="15" t="s">
         <v>41</v>
       </c>
@@ -1008,7 +1016,9 @@
       <c r="A22" s="1">
         <v>26</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="1">
+        <v>2</v>
+      </c>
       <c r="C22" s="15" t="s">
         <v>42</v>
       </c>
@@ -1020,7 +1030,9 @@
       <c r="A23" s="1">
         <v>27</v>
       </c>
-      <c r="B23" s="1"/>
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
       <c r="C23" s="15" t="s">
         <v>43</v>
       </c>
@@ -1032,7 +1044,9 @@
       <c r="A24" s="1">
         <v>28</v>
       </c>
-      <c r="B24" s="1"/>
+      <c r="B24" s="1">
+        <v>3</v>
+      </c>
       <c r="C24" s="15" t="s">
         <v>44</v>
       </c>
@@ -1044,7 +1058,9 @@
       <c r="A25" s="1">
         <v>29</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
       <c r="C25" s="15" t="s">
         <v>45</v>
       </c>
@@ -1056,7 +1072,9 @@
       <c r="A26" s="1">
         <v>30</v>
       </c>
-      <c r="B26" s="1"/>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
       <c r="C26" s="15" t="s">
         <v>46</v>
       </c>
@@ -1068,7 +1086,9 @@
       <c r="A27" s="1">
         <v>31</v>
       </c>
-      <c r="B27" s="1"/>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
       <c r="C27" s="15" t="s">
         <v>47</v>
       </c>

</xml_diff>